<commit_message>
Updates to professional service
</commit_message>
<xml_diff>
--- a/data/admin.xlsx
+++ b/data/admin.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ueanorwich-my.sharepoint.com/personal/hpd08ucu_uea_ac_uk/Documents/CV/jy_CV/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ueanorwich-my.sharepoint.com/personal/hpd08ucu_uea_ac_uk/Documents/CV/PL_CV/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{C47A848C-0516-4D36-AFC8-4480E99B5B5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{09AC686D-8BCA-42E8-9F3F-65A91D6E37ED}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{C47A848C-0516-4D36-AFC8-4480E99B5B5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{6C9CCC1C-A7CB-46ED-923D-0092589EC5CE}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-4965" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>what</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t xml:space="preserve">School of Biological Sciences </t>
+  </si>
+  <si>
+    <t>Faculty of Science</t>
+  </si>
+  <si>
+    <t>Statistician - Animal Welfare Ethical Review Body</t>
   </si>
 </sst>
 </file>
@@ -893,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -943,6 +949,20 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>